<commit_message>
Fix node version for LTS
</commit_message>
<xml_diff>
--- a/build-pipeline.xlsx
+++ b/build-pipeline.xlsx
@@ -90,9 +90,6 @@
     <t>v6.3</t>
   </si>
   <si>
-    <t>v4.7</t>
-  </si>
-  <si>
     <t>npm</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>test:zip</t>
+  </si>
+  <si>
+    <t>v4.4</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,7 +499,7 @@
     <col min="7" max="7" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>14</v>
@@ -522,7 +522,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>15</v>
@@ -531,7 +531,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -539,7 +539,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>16</v>
@@ -548,7 +548,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -556,35 +556,35 @@
     </row>
     <row r="4" spans="1:7" ht="42" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -592,7 +592,7 @@
     </row>
     <row r="6" spans="1:7" ht="42" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>18</v>
@@ -601,14 +601,14 @@
         <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="84" x14ac:dyDescent="0.2">
@@ -616,16 +616,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>13</v>
@@ -637,20 +637,20 @@
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -658,13 +658,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>

</xml_diff>

<commit_message>
Removing support for node v0.10 and v0.12 node v0.10 was deprecated Oct 1; v0.12 will be deprecated in Dec.
</commit_message>
<xml_diff>
--- a/build-pipeline.xlsx
+++ b/build-pipeline.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Notes</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>v5.12</t>
-  </si>
-  <si>
-    <t>v6.3</t>
   </si>
   <si>
     <t>npm</t>
@@ -135,6 +132,15 @@
   </si>
   <si>
     <t>v4.4</t>
+  </si>
+  <si>
+    <t>v6.9.1</t>
+  </si>
+  <si>
+    <t>mb version</t>
+  </si>
+  <si>
+    <t>EOL v1.7</t>
   </si>
 </sst>
 </file>
@@ -172,12 +178,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -192,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -205,6 +217,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,201 +502,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" ht="42" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="42" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="42" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="84" x14ac:dyDescent="0.2">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="84" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" ht="42" x14ac:dyDescent="0.2">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="42" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="E8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="5"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated ruby dependency version
</commit_message>
<xml_diff>
--- a/build-pipeline.xlsx
+++ b/build-pipeline.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Notes</t>
   </si>
@@ -137,10 +137,13 @@
     <t>v6.9.1</t>
   </si>
   <si>
-    <t>mb version</t>
-  </si>
-  <si>
-    <t>EOL v1.7</t>
+    <t>7.1.0</t>
+  </si>
+  <si>
+    <t>EOL mb version</t>
+  </si>
+  <si>
+    <t>v1.7</t>
   </si>
 </sst>
 </file>
@@ -204,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -225,6 +228,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +520,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" customWidth="1"/>
@@ -522,8 +531,8 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>14</v>
@@ -548,8 +557,8 @@
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>31</v>
+      <c r="B2" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>15</v>
@@ -568,8 +577,8 @@
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>31</v>
+      <c r="B3" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>16</v>
@@ -588,7 +597,7 @@
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="4" t="s">
         <v>28</v>
       </c>
@@ -610,7 +619,7 @@
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
@@ -626,9 +635,9 @@
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>12</v>
@@ -648,9 +657,9 @@
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>5</v>
@@ -670,7 +679,7 @@
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="4" t="s">
         <v>28</v>
       </c>
@@ -692,7 +701,7 @@
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="4" t="s">
         <v>28</v>
       </c>

</xml_diff>